<commit_message>
Actualised test scenario by test reproduction steps
</commit_message>
<xml_diff>
--- a/ScenariuszTestow.xlsx
+++ b/ScenariuszTestow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KUBA\PROJECTS\TestujSystell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5C6E6C-7F1A-4729-BD90-4D2CE4C392D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230C7C42-AA77-42C5-B6FE-06770CC0EC05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Testy jednostkowe</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>Testy wydajnościowe i obciążeniowe</t>
+  </si>
+  <si>
+    <t>Wejście na stronę -&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wejście na stronę -&gt; otwarcie menu z wyborem języka -&gt; wybranie języka angielskiego -&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wykonanie następujących czynności 10 razy w tym samym momencie: wejście na stronę -&gt; kliknięcie w link "Więcej postów" -&gt; </t>
   </si>
 </sst>
 </file>
@@ -171,20 +180,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,6 +239,11 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -268,12 +284,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="hair">
+        <color auto="1"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -283,12 +305,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -296,59 +318,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="3" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="3" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="3" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="3" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="3" xfId="8" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="3" xfId="8" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="0" xfId="8" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="20% - Accent1" xfId="7" builtinId="30"/>
-    <cellStyle name="60% - Accent1" xfId="8" builtinId="32"/>
-    <cellStyle name="Accent1" xfId="6" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="6" builtinId="30"/>
+    <cellStyle name="60% - Accent1" xfId="7" builtinId="32"/>
+    <cellStyle name="Accent1" xfId="5" builtinId="29"/>
+    <cellStyle name="Calculation" xfId="8" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Warning Text" xfId="5" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -629,7 +666,7 @@
   <dimension ref="B2:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,45 +674,52 @@
     <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31" style="1" customWidth="1"/>
     <col min="6" max="6" width="86" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-    </row>
-    <row r="3" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="13"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E5" s="2"/>
-      <c r="F5" s="3" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="2"/>
@@ -684,14 +728,21 @@
       <c r="B6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="13"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E7" s="2"/>
-      <c r="F7" s="4" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18" t="s">
         <v>3</v>
       </c>
     </row>
@@ -699,39 +750,54 @@
       <c r="B8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F9" s="5" t="s">
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="s">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-    </row>
-    <row r="11" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="13"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E12" s="2"/>
-      <c r="F12" s="3" t="s">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15" t="s">
         <v>9</v>
       </c>
     </row>
@@ -739,13 +805,21 @@
       <c r="B13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="13"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="2:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="6" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -753,69 +827,89 @@
       <c r="B15" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="C15" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="13"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F16" s="6" t="s">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="7" t="s">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="8" t="s">
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-    </row>
-    <row r="19" spans="2:6" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="12" t="s">
+      <c r="C19" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="13"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="3" t="s">
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="12"/>
+      <c r="C20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="15" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="19">
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="C17:F17"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="C19:D19"/>
     <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="C3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>